<commit_message>
Metodos añadidos en permisos, y organizacion
</commit_message>
<xml_diff>
--- a/CRUD - DICCIONARIO- DIEÑO MER/CRUD.xlsx
+++ b/CRUD - DICCIONARIO- DIEÑO MER/CRUD.xlsx
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +233,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +262,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF6FA8DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
@@ -282,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -298,6 +322,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,10 +694,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -732,10 +765,10 @@
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="4"/>
@@ -763,10 +796,10 @@
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4"/>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -792,10 +825,10 @@
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4"/>
+      <c r="B6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -821,10 +854,10 @@
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4"/>
+      <c r="B7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="10"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -850,10 +883,10 @@
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -921,8 +954,8 @@
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
@@ -950,8 +983,8 @@
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
@@ -979,8 +1012,8 @@
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="4"/>
@@ -1008,8 +1041,8 @@
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1037,8 +1070,8 @@
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1066,8 +1099,8 @@
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="4" t="s">
         <v>30</v>
       </c>
@@ -1095,8 +1128,8 @@
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="4" t="s">
         <v>30</v>
       </c>
@@ -1124,8 +1157,8 @@
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
         <v>28</v>
@@ -1153,8 +1186,8 @@
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
         <v>28</v>
@@ -1182,8 +1215,8 @@
       <c r="A18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1211,8 +1244,8 @@
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
         <v>30</v>
@@ -1248,8 +1281,8 @@
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
         <v>30</v>
@@ -1277,8 +1310,8 @@
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1306,8 +1339,8 @@
       <c r="A22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
@@ -1339,10 +1372,10 @@
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="4"/>
+      <c r="B23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="10"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1368,8 +1401,8 @@
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="4"/>
@@ -1397,10 +1430,10 @@
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1434,8 +1467,8 @@
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
@@ -1469,8 +1502,8 @@
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="4"/>
@@ -1508,8 +1541,8 @@
       <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="4"/>
@@ -1547,8 +1580,8 @@
       <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="4"/>
@@ -1586,8 +1619,8 @@
       <c r="A30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="4"/>
@@ -1623,8 +1656,8 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1650,8 +1683,8 @@
       <c r="A32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1675,8 +1708,8 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1700,10 +1733,10 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">

</xml_diff>